<commit_message>
fix details in MOVPE Ga2O3
</commit_message>
<xml_diff>
--- a/movpe_IKZ_Ga2O3/Substrate_GaO.xlsx
+++ b/movpe_IKZ_Ga2O3/Substrate_GaO.xlsx
@@ -220,7 +220,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">An unique ID given to each substrate: 
+      <t xml:space="preserve">A unique ID given to each substrate: 
 Ex. MgC121_4deg_P76189_10x10_B4_(BOX1)
 Mg: semi-insulating
 C121: Crystal number 121
@@ -589,7 +589,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="61">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -602,8 +602,8 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -706,7 +706,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -786,7 +786,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -798,7 +798,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -826,11 +826,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -917,7 +913,7 @@
   </sheetPr>
   <dimension ref="A1:ALT18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="280" zoomScaleNormal="280" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G24" activeCellId="0" sqref="G24"/>
     </sheetView>
   </sheetViews>
@@ -929,8 +925,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="10.82"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1007" min="9" style="1" width="9.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1008" min="1008" style="3" width="11.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1009" style="0" width="11.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1008" min="1008" style="1" width="11.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1009" style="3" width="11.54"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -938,14 +934,14 @@
         <v>0</v>
       </c>
       <c r="B1" s="5"/>
-      <c r="ALT1" s="3"/>
+      <c r="ALT1" s="1"/>
     </row>
     <row r="2" s="6" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="7"/>
-      <c r="ALT2" s="3"/>
+      <c r="ALT2" s="1"/>
     </row>
     <row r="3" s="11" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
@@ -972,7 +968,7 @@
       <c r="H3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="ALT3" s="3"/>
+      <c r="ALT3" s="1"/>
     </row>
     <row r="4" s="13" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
@@ -985,7 +981,7 @@
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
       <c r="H4" s="12"/>
-      <c r="ALT4" s="3"/>
+      <c r="ALT4" s="1"/>
     </row>
     <row r="5" s="8" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
@@ -1012,7 +1008,7 @@
       <c r="H5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="ALT5" s="3"/>
+      <c r="ALT5" s="1"/>
     </row>
     <row r="6" s="14" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="14" t="s">
@@ -1025,7 +1021,7 @@
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
       <c r="H6" s="16"/>
-      <c r="ALT6" s="3"/>
+      <c r="ALT6" s="1"/>
     </row>
     <row r="7" s="17" customFormat="true" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
@@ -1052,7 +1048,7 @@
       <c r="H7" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="ALT7" s="3"/>
+      <c r="ALT7" s="1"/>
     </row>
     <row r="8" s="18" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="18" t="s">
@@ -1065,7 +1061,7 @@
       <c r="F8" s="20"/>
       <c r="G8" s="20"/>
       <c r="H8" s="20"/>
-      <c r="ALT8" s="3"/>
+      <c r="ALT8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="21" t="s">
@@ -1204,8 +1200,8 @@
   </sheetPr>
   <dimension ref="A1:AMO30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P7" colorId="64" zoomScale="280" zoomScaleNormal="280" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V15" activeCellId="0" sqref="V15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U21" activeCellId="0" sqref="U21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.18359375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1226,9 +1222,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="27" width="11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="19" style="27" width="10.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="27" width="21.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="27" width="14.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="27" width="14.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="27" width="10.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="27" width="12.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="27" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="27" width="9.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="27" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="27" width="7.52"/>
@@ -1244,7 +1240,7 @@
       </c>
       <c r="F1" s="31"/>
       <c r="AMN1" s="29"/>
-      <c r="AMO1" s="0"/>
+      <c r="AMO1" s="3"/>
     </row>
     <row r="2" s="32" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="32" t="s">
@@ -1252,7 +1248,7 @@
       </c>
       <c r="F2" s="33"/>
       <c r="AMN2" s="29"/>
-      <c r="AMO2" s="0"/>
+      <c r="AMO2" s="3"/>
     </row>
     <row r="3" s="37" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="34" t="s">
@@ -1340,7 +1336,7 @@
         <v>5</v>
       </c>
       <c r="AMN3" s="29"/>
-      <c r="AMO3" s="0"/>
+      <c r="AMO3" s="3"/>
     </row>
     <row r="4" s="39" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="32" t="s">
@@ -1374,7 +1370,7 @@
       <c r="AA4" s="38"/>
       <c r="AB4" s="38"/>
       <c r="AMN4" s="29"/>
-      <c r="AMO4" s="0"/>
+      <c r="AMO4" s="3"/>
     </row>
     <row r="5" s="34" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="34" t="s">
@@ -1462,7 +1458,7 @@
         <v>9</v>
       </c>
       <c r="AMN5" s="29"/>
-      <c r="AMO5" s="0"/>
+      <c r="AMO5" s="3"/>
     </row>
     <row r="6" s="41" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="41" t="s">
@@ -1480,9 +1476,9 @@
       <c r="AA6" s="43"/>
       <c r="AB6" s="43"/>
       <c r="AMN6" s="29"/>
-      <c r="AMO6" s="0"/>
-    </row>
-    <row r="7" s="45" customFormat="true" ht="216.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AMO6" s="3"/>
+    </row>
+    <row r="7" s="45" customFormat="true" ht="183.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="34" t="s">
         <v>36</v>
       </c>
@@ -1568,7 +1564,7 @@
         <v>59</v>
       </c>
       <c r="AMN7" s="29"/>
-      <c r="AMO7" s="0"/>
+      <c r="AMO7" s="3"/>
     </row>
     <row r="8" s="46" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="46" t="s">
@@ -1586,7 +1582,7 @@
       <c r="AA8" s="48"/>
       <c r="AB8" s="48"/>
       <c r="AMN8" s="29"/>
-      <c r="AMO8" s="0"/>
+      <c r="AMO8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="49" t="s">
@@ -1741,10 +1737,10 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="V10" s="59" t="n">
+      <c r="V10" s="57" t="n">
         <v>900</v>
       </c>
-      <c r="W10" s="59" t="n">
+      <c r="W10" s="57" t="n">
         <v>60</v>
       </c>
       <c r="X10" s="58" t="n">
@@ -1767,14 +1763,14 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="60"/>
-      <c r="B11" s="61"/>
+      <c r="A11" s="59"/>
+      <c r="B11" s="60"/>
       <c r="I11" s="55"/>
       <c r="L11" s="55"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="61"/>
-      <c r="B12" s="61"/>
+      <c r="A12" s="60"/>
+      <c r="B12" s="60"/>
       <c r="I12" s="55"/>
       <c r="L12" s="55"/>
     </row>

</xml_diff>